<commit_message>
Update Leave Card 8/7/2023 4:34 PM
</commit_message>
<xml_diff>
--- a/BRON, FLORENCIO.xlsx
+++ b/BRON, FLORENCIO.xlsx
@@ -1,48 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017772F5-0115-41A3-A625-735F4ADFDFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="CONVERTION" sheetId="3" r:id="rId3"/>
+    <sheet name="2018 LEAVE CREDITS" sheetId="1" r:id="rId2"/>
+    <sheet name="2017 LEAVE BALANCE" sheetId="5" r:id="rId3"/>
+    <sheet name="CONVERTION" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="BALANCE_1" localSheetId="2">[1]!Table1[[#Headers],[BALANCE]]</definedName>
+    <definedName name="BALANCE_1" localSheetId="2">Table13[[#Headers],[BALANCE]]</definedName>
+    <definedName name="BALANCE_1" localSheetId="3">[1]!Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet1!$1:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>PERIOD</t>
   </si>
@@ -226,11 +222,50 @@
   <si>
     <t>7/16,17/2023</t>
   </si>
+  <si>
+    <t>6/5,6/2018</t>
+  </si>
+  <si>
+    <t>6/17,20/2018</t>
+  </si>
+  <si>
+    <t>9/15,16/2018</t>
+  </si>
+  <si>
+    <t>1/12-13/2019</t>
+  </si>
+  <si>
+    <t>8/3,4/2019</t>
+  </si>
+  <si>
+    <t>10/21,22/2019</t>
+  </si>
+  <si>
+    <t>12/2,3/2019</t>
+  </si>
+  <si>
+    <t>2/11,12/2020</t>
+  </si>
+  <si>
+    <t>9/20,21/2020</t>
+  </si>
+  <si>
+    <t>10/5,7/2020</t>
+  </si>
+  <si>
+    <t>1/18,19/2021</t>
+  </si>
+  <si>
+    <t>7/9,10/2021</t>
+  </si>
+  <si>
+    <t>FL(4-0-0)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -461,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -639,11 +674,255 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="30">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -918,7 +1197,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +1240,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,7 +1304,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1085,7 +1364,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1151,7 +1430,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1214,7 +1493,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1312,7 +1591,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1371,7 +1650,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1715,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1479,7 +1758,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1554,7 +1833,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1740,7 +2019,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1806,7 +2085,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1864,7 +2143,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1930,7 +2209,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1986,7 +2265,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2061,7 +2340,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2104,7 +2383,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2170,7 +2449,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2226,7 +2505,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2305,7 +2584,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2322,25 +2601,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altText="BALANCE_2"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{27A6A43E-4275-4FB4-8365-760D3AE71C74}" name="Table13" displayName="Table13" ref="A8:K97" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{2A2BE981-3017-4606-8823-8A12743EAEB8}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A34E99D4-E4B0-4045-B22F-DD5963A78228}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CE8E396D-CCE6-4335-9527-CC70087B5727}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{327A410C-1410-43BF-BF53-1D5DE84F6124}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{422A393A-DC3C-4C3C-AFA4-D4F06A5F0480}" name="BALANCE" dataDxfId="6">
+      <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{81324F36-AAEA-48EB-BC08-C825E1D2560D}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{CA02FCC7-7792-4EDB-8E01-16746C8C03C8}" name="EARNED " dataDxfId="4">
+      <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7B55E07B-8705-4648-AB56-AA1CC2461551}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{B5BDAE25-BD90-4AB5-AD0F-C76BB946D49A}" name="BALANCE " dataDxfId="2">
+      <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{218B10EE-F4E6-4FE5-B709-7408379C6E08}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{A27937B5-AED7-4FDD-B288-776332DF9490}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2647,7 +2956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2657,7 +2966,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2665,34 +2974,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A68" activePane="bottomLeft"/>
-      <selection activeCell="F3" sqref="F3:G3"/>
-      <selection pane="bottomLeft" activeCell="J83" sqref="J83"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A85" activePane="bottomLeft"/>
+      <selection activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2713,7 +3022,7 @@
       <c r="J2" s="52"/>
       <c r="K2" s="53"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2733,7 +3042,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2753,7 +3062,7 @@
       <c r="J4" s="52"/>
       <c r="K4" s="53"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2761,7 +3070,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2774,7 +3083,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="50" t="s">
@@ -2791,7 +3100,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2826,7 +3135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2834,8 +3143,8 @@
       <c r="C9" s="13"/>
       <c r="D9" s="11"/>
       <c r="E9" s="13">
-        <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>64.5</v>
+        <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])</f>
+        <v>58.75</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2844,13 +3153,13 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="13">
-        <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>76.5</v>
+        <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])</f>
+        <v>83.75</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +3181,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -2892,7 +3201,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -2912,7 +3221,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -2932,7 +3241,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -2952,7 +3261,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -2972,7 +3281,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -2992,7 +3301,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3012,7 +3321,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3032,7 +3341,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3052,7 +3361,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3072,7 +3381,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3092,7 +3401,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3116,7 +3425,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
@@ -3134,7 +3443,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3154,7 +3463,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3174,7 +3483,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3194,7 +3503,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3214,7 +3523,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3234,7 +3543,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3254,7 +3563,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -3274,7 +3583,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -3294,7 +3603,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -3314,7 +3623,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -3334,7 +3643,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -3354,7 +3663,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -3378,7 +3687,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>47</v>
       </c>
@@ -3396,7 +3705,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -3416,7 +3725,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -3436,7 +3745,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -3456,7 +3765,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -3476,7 +3785,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -3496,7 +3805,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -3516,7 +3825,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -3536,7 +3845,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -3556,7 +3865,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -3576,7 +3885,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -3596,7 +3905,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -3616,7 +3925,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -3640,7 +3949,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="48" t="s">
         <v>48</v>
       </c>
@@ -3658,7 +3967,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -3678,7 +3987,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -3698,7 +4007,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -3718,7 +4027,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -3738,7 +4047,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -3758,7 +4067,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -3778,7 +4087,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -3798,7 +4107,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -3818,7 +4127,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -3838,7 +4147,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -3858,7 +4167,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -3878,7 +4187,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -3888,7 +4197,9 @@
       <c r="C61" s="13">
         <v>1.25</v>
       </c>
-      <c r="D61" s="39"/>
+      <c r="D61" s="39">
+        <v>5</v>
+      </c>
       <c r="E61" s="9"/>
       <c r="F61" s="20"/>
       <c r="G61" s="13">
@@ -3900,7 +4211,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="48" t="s">
         <v>49</v>
       </c>
@@ -3918,7 +4229,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -3938,7 +4249,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -3958,7 +4269,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -3978,7 +4289,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40">
         <v>44652</v>
       </c>
@@ -3998,7 +4309,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40">
         <v>44682</v>
       </c>
@@ -4018,7 +4329,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40">
         <v>44713</v>
       </c>
@@ -4038,13 +4349,11 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">
         <v>44743</v>
       </c>
-      <c r="B69" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="B69" s="20"/>
       <c r="C69" s="13">
         <v>1.25</v>
       </c>
@@ -4055,16 +4364,12 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H69" s="39">
-        <v>2</v>
-      </c>
+      <c r="H69" s="39"/>
       <c r="I69" s="9"/>
       <c r="J69" s="11"/>
-      <c r="K69" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="20"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40">
         <v>44774</v>
       </c>
@@ -4084,7 +4389,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
         <v>44805</v>
       </c>
@@ -4110,7 +4415,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40">
         <v>44835</v>
       </c>
@@ -4130,13 +4435,11 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40">
         <v>44866</v>
       </c>
-      <c r="B73" s="20" t="s">
-        <v>51</v>
-      </c>
+      <c r="B73" s="20"/>
       <c r="C73" s="13">
         <v>1.25</v>
       </c>
@@ -4147,16 +4450,12 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H73" s="39">
-        <v>2</v>
-      </c>
+      <c r="H73" s="39"/>
       <c r="I73" s="9"/>
       <c r="J73" s="11"/>
-      <c r="K73" s="20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="20"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
         <v>44896</v>
       </c>
@@ -4180,13 +4479,15 @@
         <v>44913</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B75" s="20"/>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="40"/>
+      <c r="B75" s="20" t="s">
+        <v>73</v>
+      </c>
       <c r="C75" s="13"/>
-      <c r="D75" s="39"/>
+      <c r="D75" s="39">
+        <v>4</v>
+      </c>
       <c r="E75" s="9"/>
       <c r="F75" s="20"/>
       <c r="G75" s="13" t="str">
@@ -4196,31 +4497,29 @@
       <c r="H75" s="39"/>
       <c r="I75" s="9"/>
       <c r="J75" s="11"/>
-      <c r="K75" s="20"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="40">
-        <v>44927</v>
+      <c r="K75" s="49"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="48" t="s">
+        <v>55</v>
       </c>
       <c r="B76" s="20"/>
-      <c r="C76" s="13">
-        <v>1.25</v>
-      </c>
+      <c r="C76" s="13"/>
       <c r="D76" s="39"/>
       <c r="E76" s="9"/>
       <c r="F76" s="20"/>
-      <c r="G76" s="13">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v>1.25</v>
+      <c r="G76" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
       </c>
       <c r="H76" s="39"/>
       <c r="I76" s="9"/>
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40">
-        <v>44958</v>
+        <v>44927</v>
       </c>
       <c r="B77" s="20"/>
       <c r="C77" s="13">
@@ -4238,13 +4537,11 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40">
-        <v>44986</v>
-      </c>
-      <c r="B78" s="20" t="s">
-        <v>56</v>
-      </c>
+        <v>44958</v>
+      </c>
+      <c r="B78" s="20"/>
       <c r="C78" s="13">
         <v>1.25</v>
       </c>
@@ -4255,38 +4552,32 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H78" s="39">
-        <v>1</v>
-      </c>
+      <c r="H78" s="39"/>
       <c r="I78" s="9"/>
       <c r="J78" s="11"/>
-      <c r="K78" s="49">
-        <v>44989</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="40"/>
-      <c r="B79" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="13"/>
-      <c r="D79" s="39">
-        <v>2</v>
-      </c>
+      <c r="K78" s="20"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="40">
+        <v>44986</v>
+      </c>
+      <c r="B79" s="20"/>
+      <c r="C79" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D79" s="39"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
-      <c r="G79" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G79" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H79" s="39"/>
       <c r="I79" s="9"/>
       <c r="J79" s="11"/>
-      <c r="K79" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K79" s="49"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40">
         <v>45017</v>
       </c>
@@ -4306,7 +4597,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40">
         <v>45047</v>
       </c>
@@ -4326,13 +4617,11 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40">
         <v>45078</v>
       </c>
-      <c r="B82" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="B82" s="20"/>
       <c r="C82" s="13">
         <v>1.25</v>
       </c>
@@ -4343,29 +4632,27 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v>1.25</v>
       </c>
-      <c r="H82" s="39">
-        <v>1</v>
-      </c>
+      <c r="H82" s="39"/>
       <c r="I82" s="9"/>
       <c r="J82" s="11"/>
-      <c r="K82" s="49">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K82" s="49"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40">
         <v>45108</v>
       </c>
       <c r="B83" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C83" s="13"/>
+      <c r="C83" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D83" s="39"/>
       <c r="E83" s="9"/>
       <c r="F83" s="20"/>
-      <c r="G83" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G83" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H83" s="39"/>
       <c r="I83" s="9"/>
@@ -4374,7 +4661,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40">
         <v>45139</v>
       </c>
@@ -4392,7 +4679,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40">
         <v>45170</v>
       </c>
@@ -4410,7 +4697,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40">
         <v>45200</v>
       </c>
@@ -4428,7 +4715,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40">
         <v>45231</v>
       </c>
@@ -4446,7 +4733,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40">
         <v>45261</v>
       </c>
@@ -4464,7 +4751,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4480,7 +4767,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4496,7 +4783,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4512,7 +4799,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4528,7 +4815,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4544,7 +4831,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4560,7 +4847,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4576,7 +4863,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4592,7 +4879,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4608,7 +4895,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4624,7 +4911,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4640,7 +4927,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4656,7 +4943,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4672,7 +4959,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4688,7 +4975,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4704,7 +4991,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4720,7 +5007,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4736,7 +5023,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4752,7 +5039,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4768,7 +5055,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4784,7 +5071,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4800,7 +5087,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4816,7 +5103,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4832,7 +5119,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4848,7 +5135,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4864,7 +5151,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4880,7 +5167,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4896,7 +5183,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4912,7 +5199,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4928,7 +5215,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4944,7 +5231,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4960,7 +5247,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4976,7 +5263,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -4992,7 +5279,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5008,7 +5295,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5024,7 +5311,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5040,7 +5327,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5056,7 +5343,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5072,7 +5359,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5088,7 +5375,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5104,7 +5391,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5120,7 +5407,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="41"/>
       <c r="B130" s="15"/>
       <c r="C130" s="42"/>
@@ -5151,10 +5438,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5177,28 +5464,1944 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A08D049-4E26-45A9-86C8-9F4D0411F27A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:K97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" activePane="bottomLeft"/>
+      <selection activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="25"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="57">
+        <v>43101</v>
+      </c>
+      <c r="G3" s="52"/>
+      <c r="H3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="26"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="26"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="H5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="27"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="13">
+        <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
+        <v>168.584</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="13">
+        <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
+        <v>30.75</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="40">
+        <v>43221</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H11" s="39">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="49">
+        <v>43241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="40">
+        <v>43252</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H12" s="39">
+        <v>2</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="40"/>
+      <c r="B13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H13" s="39">
+        <v>2</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H14" s="39">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="49">
+        <v>43298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H15" s="39">
+        <v>2</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="40"/>
+      <c r="B16" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H16" s="39">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="49">
+        <v>43386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="40">
+        <v>43405</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="49">
+        <v>43411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="40">
+        <v>43435</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H18" s="39">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="49">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H19" s="39"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="49"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="61">
+        <v>43466</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H20" s="39">
+        <v>2</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="61">
+        <v>43525</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H21" s="39">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="49">
+        <v>43535</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="61">
+        <v>43556</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H22" s="39">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="49">
+        <v>43577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="61"/>
+      <c r="B23" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H23" s="39">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="49">
+        <v>43605</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="61">
+        <v>43647</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H24" s="39">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="49">
+        <v>43669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="61"/>
+      <c r="B25" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H25" s="39">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="49">
+        <v>43663</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="61">
+        <v>43678</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H26" s="39">
+        <v>2</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="61"/>
+      <c r="B27" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H27" s="39">
+        <v>1</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="49">
+        <v>43704</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="61">
+        <v>43739</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="39">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H28" s="39"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="61">
+        <v>43770</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H29" s="39">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="49">
+        <v>43780</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="61">
+        <v>43800</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H30" s="39">
+        <v>2</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H31" s="39"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="49"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="61">
+        <v>43831</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H32" s="39">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="49">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="61">
+        <v>43862</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H33" s="39">
+        <v>2</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="61">
+        <v>44013</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H34" s="39">
+        <v>1</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="49">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="61">
+        <v>44044</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H35" s="39">
+        <v>1</v>
+      </c>
+      <c r="I35" s="9"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="49">
+        <v>44068</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="61">
+        <v>44075</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H36" s="39">
+        <v>2</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="61">
+        <v>44105</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H37" s="39">
+        <v>2</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H38" s="39"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="49"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="61">
+        <v>44197</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H39" s="39">
+        <v>2</v>
+      </c>
+      <c r="I39" s="9"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="61">
+        <v>44256</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H40" s="39"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="49">
+        <v>44263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="61">
+        <v>44378</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H41" s="39">
+        <v>2</v>
+      </c>
+      <c r="I41" s="9"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H42" s="39"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="20"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="40">
+        <v>44743</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H43" s="39">
+        <v>2</v>
+      </c>
+      <c r="I43" s="9"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="40">
+        <v>44866</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H44" s="39">
+        <v>2</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="40">
+        <v>44896</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H45" s="39"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="49">
+        <v>44913</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H46" s="39"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="20"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="40">
+        <v>44986</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H47" s="39">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="49">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="40"/>
+      <c r="B48" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="39">
+        <v>2</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H48" s="39"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="40">
+        <v>45078</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H49" s="39">
+        <v>1</v>
+      </c>
+      <c r="I49" s="9"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="49">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="40">
+        <v>45108</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H50" s="39"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="40">
+        <v>45139</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H51" s="39"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="20"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="40">
+        <v>45170</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H52" s="39"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="20"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="40">
+        <v>45200</v>
+      </c>
+      <c r="B53" s="20"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H53" s="39"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="20"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="40">
+        <v>45231</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H54" s="39"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="20"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="40">
+        <v>45261</v>
+      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H55" s="39"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="20"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="40"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H56" s="39"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="20"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="40"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H57" s="39"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="20"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="40"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H58" s="39"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="20"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="40"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H59" s="39"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="20"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="40"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H60" s="39"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="20"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="40"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H61" s="39"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="20"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="40"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H62" s="39"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="20"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="40"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H63" s="39"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="20"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="40"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H64" s="39"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="20"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="40"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H65" s="39"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="20"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="40"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H66" s="39"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="20"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="40"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H67" s="39"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="20"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="40"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H68" s="39"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="20"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="40"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H69" s="39"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="20"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="40"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H70" s="39"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="20"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="40"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H71" s="39"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="20"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="40"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H72" s="39"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="20"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="40"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H73" s="39"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="20"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="40"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H74" s="39"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="20"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="40"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H75" s="39"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="20"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="40"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H76" s="39"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="20"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="40"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H77" s="39"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="20"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="40"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H78" s="39"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="20"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="40"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H79" s="39"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="20"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="40"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H80" s="39"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="20"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="40"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H81" s="39"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="20"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="40"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H82" s="39"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="20"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="40"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H83" s="39"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="20"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="40"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H84" s="39"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="11"/>
+      <c r="K84" s="20"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="40"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H85" s="39"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="20"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="40"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H86" s="39"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="11"/>
+      <c r="K86" s="20"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="40"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H87" s="39"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="20"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="40"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="39"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H88" s="39"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="20"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="40"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H89" s="39"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="20"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="40"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H90" s="39"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="11"/>
+      <c r="K90" s="20"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" s="40"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H91" s="39"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="20"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="40"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H92" s="39"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="20"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="40"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H93" s="39"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="20"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" s="40"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H94" s="39"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="20"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" s="40"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H95" s="39"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="11"/>
+      <c r="K95" s="20"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96" s="40"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H96" s="39"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="11"/>
+      <c r="K96" s="20"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" s="41"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="43"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="42" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H97" s="43"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{541EAEE8-BFBF-4843-A075-DBFC3A2ADA98}">
+      <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{332E9606-8D3E-4CE9-B3F3-E33A13D655CC}">
+      <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="89" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"-,Bold"&amp;12REPUBLIC OF THE PHILIPPINES
+CITY OF TAGAYTAY
+EMPLOYEE'S LEAVE CARD</oddHeader>
+    <oddFooter>&amp;L
+PREPARED BY: ___________________
+DATE: &amp;D, &amp;T&amp;C
+CERTIFIED CORRECT BY: &amp;UALMA A. MALABANAN&amp;U
+                                   HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5211,7 +7414,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5240,9 +7443,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>172.584</v>
+      </c>
+      <c r="B3" s="11">
+        <v>72.75</v>
+      </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -5260,17 +7467,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5291,7 +7498,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5318,7 +7525,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5344,7 +7551,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5370,7 +7577,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5396,7 +7603,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5422,7 +7629,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5448,7 +7655,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5474,7 +7681,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5500,7 +7707,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5520,7 +7727,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5540,7 +7747,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5560,7 +7767,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5581,7 +7788,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5602,7 +7809,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5623,7 +7830,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5644,7 +7851,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5665,7 +7872,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5686,7 +7893,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5707,7 +7914,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5728,7 +7935,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5749,7 +7956,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5770,7 +7977,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5791,7 +7998,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5812,7 +8019,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5833,7 +8040,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5854,7 +8061,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5875,7 +8082,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -5896,7 +8103,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -5917,7 +8124,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -5938,7 +8145,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -5959,7 +8166,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -5980,7 +8187,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -5989,7 +8196,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -5998,7 +8205,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -6007,7 +8214,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -6016,7 +8223,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -6025,7 +8232,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -6034,7 +8241,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -6043,7 +8250,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -6052,7 +8259,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -6061,7 +8268,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6070,7 +8277,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6079,7 +8286,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6088,7 +8295,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6097,7 +8304,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6106,7 +8313,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6115,7 +8322,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6124,7 +8331,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6133,7 +8340,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6142,7 +8349,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6151,7 +8358,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6160,7 +8367,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6169,7 +8376,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6178,7 +8385,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6187,7 +8394,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6196,7 +8403,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6205,7 +8412,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6214,7 +8421,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6223,7 +8430,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6232,7 +8439,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6241,7 +8448,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>